<commit_message>
Renaming terms in tabular-defined schemas and table metadata:
Schema
  Model --> Class

Table metadata (also simplifies the key names and aligns it with the comparatively simpler keys Description and Date)
  ModelId --> Id
  ModelName --> Name
  TableType --> Type
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data_copy.xlsx
+++ b/examples/biochemical_models/data_copy.xlsx
@@ -7,17 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="!_Table of contents" sheetId="1" r:id="rId1"/>
-    <sheet name="!_Schema" sheetId="2" r:id="rId2"/>
-    <sheet name="!Compound" sheetId="3" r:id="rId3"/>
-    <sheet name="!Model" sheetId="4" r:id="rId4"/>
-    <sheet name="!Reaction" sheetId="5" r:id="rId5"/>
+    <sheet name="!_Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="!Compound" sheetId="2" r:id="rId2"/>
+    <sheet name="!Model" sheetId="3" r:id="rId3"/>
+    <sheet name="!Reaction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!_Schema'!$A$2:$G$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!_Table of contents'!$A$2:$C$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!Compound'!$A$2:$E$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'!Reaction'!$A$2:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!_Schema'!$A$2:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!Compound'!$A$2:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!Reaction'!$A$2:$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -38,7 +36,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Select a value from "Model:1" or blank.</t>
+          <t>Select a value from "!Model:1" or blank.</t>
         </r>
       </text>
     </comment>
@@ -160,7 +158,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Select a value from "Model:1" or blank.</t>
+          <t>Select a value from "!Model:1" or blank.</t>
         </r>
       </text>
     </comment>
@@ -255,10 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
-  <si>
-    <t>'!_Schema'!A1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
   <si>
     <t>'!Compound'!A1</t>
   </si>
@@ -269,96 +264,81 @@
     <t>'!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='TableOfContents' Description='Table of contents' Date='2019-09-23 10:00:35' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!Table</t>
+    <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!Name</t>
+  </si>
+  <si>
+    <t>!Type</t>
+  </si>
+  <si>
+    <t>!Parent</t>
+  </si>
+  <si>
+    <t>!Format</t>
+  </si>
+  <si>
+    <t>!Verbose name</t>
+  </si>
+  <si>
+    <t>!Verbose name plural</t>
   </si>
   <si>
     <t>!Description</t>
   </si>
   <si>
-    <t>!Number of objects</t>
-  </si>
-  <si>
-    <t>Schema</t>
-  </si>
-  <si>
-    <t>Table/model and column/attribute definitions</t>
-  </si>
-  <si>
     <t>Compound</t>
   </si>
   <si>
     <t>Model</t>
   </si>
   <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>identifiers</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>is_constant</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>ManyToOne</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
     <t>Reaction</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Schema' Description='Table/model and column/attribute definitions' Date='2019-09-23 10:00:35' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!Name</t>
-  </si>
-  <si>
-    <t>!Type</t>
-  </si>
-  <si>
-    <t>!Parent</t>
-  </si>
-  <si>
-    <t>!Format</t>
-  </si>
-  <si>
-    <t>!Verbose name</t>
-  </si>
-  <si>
-    <t>!Verbose name plural</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>SlugAttribute</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>identifiers</t>
-  </si>
-  <si>
-    <t>StringAttribute</t>
-  </si>
-  <si>
-    <t>is_constant</t>
-  </si>
-  <si>
-    <t>BooleanAttribute</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>ManyToOneAttribute</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>column</t>
-  </si>
-  <si>
     <t>equation</t>
   </si>
   <si>
@@ -368,7 +348,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Compound' Description='Compound' ModelName='Compound' Date='2019-09-23 10:00:35' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -425,10 +405,10 @@
     <t>kegg.compound::C00022</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Model' Description='Model' ModelName='Model' Date='2019-09-23 10:00:35' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables TableType='Data' ModelId='Reaction' Description='Reaction' ModelName='Reaction' Date='2019-09-23 10:00:35' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>
@@ -835,100 +815,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
-  <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="16384" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <f>COUNTA('!Compound'!A3:A1048576)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4">
-        <f>COUNTA('!Model'!B2:XFD2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4">
-        <f>COUNTA('!Reaction'!A3:A1048576)</f>
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:C6"/>
-  <hyperlinks>
-    <hyperlink ref="A3" location="'!_Schema'!A1" tooltip="Click to view schema" display="'!_Schema'!A1"/>
-    <hyperlink ref="A4" location="'!Compound'!A1" tooltip="Click to view compound" display="'!Compound'!A1"/>
-    <hyperlink ref="A5" location="'!Model'!A1" tooltip="Click to view model" display="'!Model'!A1"/>
-    <hyperlink ref="A6" location="'!Reaction'!A1" tooltip="Click to view reaction" display="'!Reaction'!A1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -941,7 +830,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -952,79 +841,79 @@
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.01" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1032,16 +921,16 @@
     </row>
     <row r="6" spans="1:7" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1049,16 +938,16 @@
     </row>
     <row r="7" spans="1:7" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1066,115 +955,115 @@
     </row>
     <row r="8" spans="1:7" ht="15.01" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.01" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.01" customHeight="1">
       <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1182,16 +1071,16 @@
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1199,35 +1088,35 @@
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.01" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1235,16 +1124,16 @@
     </row>
     <row r="17" spans="1:7" ht="15.01" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1252,16 +1141,16 @@
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1269,21 +1158,21 @@
     </row>
     <row r="19" spans="1:7" ht="15.01" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1315,7 +1204,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1324,33 +1213,33 @@
     </row>
     <row r="2" spans="1:5" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.01" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>1</v>
@@ -1358,16 +1247,16 @@
     </row>
     <row r="4" spans="1:5" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -1375,16 +1264,16 @@
     </row>
     <row r="5" spans="1:5" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -1392,16 +1281,16 @@
     </row>
     <row r="6" spans="1:5" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
@@ -1409,16 +1298,16 @@
     </row>
     <row r="7" spans="1:5" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>1</v>
@@ -1428,8 +1317,8 @@
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A2:E7"/>
   <dataValidations count="5">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." sqref="A3:A7">
-      <formula1>'Model'!$B$1:$XFD$1</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!Model:1&quot; or blank." sqref="A3:A7">
+      <formula1>'!Model'!$B$1:$XFD$1</formula1>
     </dataValidation>
     <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B3:B7">
       <formula1>1</formula1>
@@ -1450,7 +1339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1469,21 +1358,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -1503,7 +1392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1520,7 +1409,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1531,75 +1420,75 @@
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.01" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A2:G4"/>
   <dataValidations count="7">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;Model:1&quot; or blank." sqref="A3:A4">
-      <formula1>'Model'!$B$1:$XFD$1</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!Model:1&quot; or blank." sqref="A3:A4">
+      <formula1>'!Model'!$B$1:$XFD$1</formula1>
     </dataValidation>
     <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B3:B4">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
added additional ! to worksheet names; implemented document metadata; expanded test coverage
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data_copy.xlsx
+++ b/examples/biochemical_models/data_copy.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="!_Schema" sheetId="1" r:id="rId1"/>
-    <sheet name="!Compound" sheetId="2" r:id="rId2"/>
-    <sheet name="!Model" sheetId="3" r:id="rId3"/>
-    <sheet name="!Reaction" sheetId="4" r:id="rId4"/>
+    <sheet name="!!_Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="!!Compound" sheetId="2" r:id="rId2"/>
+    <sheet name="!!Model" sheetId="3" r:id="rId3"/>
+    <sheet name="!!Reaction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!_Schema'!$A$2:$G$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!Compound'!$A$2:$E$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!Reaction'!$A$2:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Schema'!$A$3:$G$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!Compound'!$A$2:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!!Reaction'!$A$2:$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -253,18 +253,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
-  <si>
-    <t>'!Compound'!A1</t>
-  </si>
-  <si>
-    <t>'!Model'!A1</t>
-  </si>
-  <si>
-    <t>'!Reaction'!A1</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
+  <si>
+    <t>'!!Compound'!A1</t>
+  </si>
+  <si>
+    <t>'!!Model'!A1</t>
+  </si>
+  <si>
+    <t>'!!Reaction'!A1</t>
+  </si>
+  <si>
+    <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-10-10 23:09:02'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -348,7 +351,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -405,10 +408,10 @@
     <t>kegg.compound::C00022</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2019-10-10 02:11:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>
@@ -815,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -840,97 +843,91 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -938,16 +935,16 @@
     </row>
     <row r="7" spans="1:7" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -955,101 +952,97 @@
     </row>
     <row r="8" spans="1:7" ht="15.01" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="15.01" customHeight="1">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.01" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.01" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.01" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.01" customHeight="1">
@@ -1057,30 +1050,34 @@
         <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15.01" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1088,52 +1085,52 @@
     </row>
     <row r="15" spans="1:7" ht="15.01" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.01" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.01" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1141,16 +1138,16 @@
     </row>
     <row r="18" spans="1:7" ht="15.01" customHeight="1">
       <c r="A18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1158,30 +1155,47 @@
     </row>
     <row r="19" spans="1:7" ht="15.01" customHeight="1">
       <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.01" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:G19"/>
+  <autoFilter ref="A3:G20"/>
   <hyperlinks>
-    <hyperlink ref="A3" location="'!Compound'!A1" tooltip="Click to view compound" display="'!Compound'!A1"/>
-    <hyperlink ref="A9" location="'!Model'!A1" tooltip="Click to view model" display="'!Model'!A1"/>
-    <hyperlink ref="A12" location="'!Reaction'!A1" tooltip="Click to view reaction" display="'!Reaction'!A1"/>
+    <hyperlink ref="A3" location="'!!Compound'!A1" tooltip="Click to view compound" display="'!!Compound'!A1"/>
+    <hyperlink ref="A9" location="'!!Model'!A1" tooltip="Click to view model" display="'!!Model'!A1"/>
+    <hyperlink ref="A12" location="'!!Reaction'!A1" tooltip="Click to view reaction" display="'!!Reaction'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1204,7 +1218,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1213,33 +1227,33 @@
     </row>
     <row r="2" spans="1:5" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.01" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>1</v>
@@ -1247,16 +1261,16 @@
     </row>
     <row r="4" spans="1:5" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -1264,16 +1278,16 @@
     </row>
     <row r="5" spans="1:5" ht="15.01" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -1281,16 +1295,16 @@
     </row>
     <row r="6" spans="1:5" ht="15.01" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
@@ -1298,16 +1312,16 @@
     </row>
     <row r="7" spans="1:5" ht="15.01" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>1</v>
@@ -1358,21 +1372,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -1409,7 +1423,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1420,67 +1434,67 @@
     </row>
     <row r="2" spans="1:7" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.01" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.01" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
organizing attributes into domain-specific modules and reducing the amount of core imported code
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data_copy.xlsx
+++ b/examples/biochemical_models/data_copy.xlsx
@@ -36,7 +36,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Select a value from "!Model:1" or blank.</t>
+          <t>Select a value from "!!Model:2" or blank.</t>
         </r>
       </text>
     </comment>
@@ -51,7 +51,7 @@
           </rPr>
           <t>Identifier
 Enter a string.
-Value must be between 1 and 63 characters.
+Value must be between 1 and 90 characters.
 Value must be unique.</t>
         </r>
       </text>
@@ -119,7 +119,7 @@
           </rPr>
           <t>Identifier
 Enter a string.
-Value must be between 1 and 63 characters.
+Value must be between 1 and 90 characters.
 Value must be unique.</t>
         </r>
       </text>
@@ -158,7 +158,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Select a value from "!Model:1" or blank.</t>
+          <t>Select a value from "!!Model:2" or blank.</t>
         </r>
       </text>
     </comment>
@@ -173,7 +173,7 @@
           </rPr>
           <t>Identifier
 Enter a string.
-Value must be between 1 and 63 characters.
+Value must be between 1 and 90 characters.
 Value must be unique.</t>
         </r>
       </text>
@@ -264,10 +264,10 @@
     <t>'!!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-10-10 23:09:02'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2020-03-05 18:09:25'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Schema' Description='Table/model and column/attribute definitions' Date='2020-03-05 18:09:25' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -351,7 +351,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Compound' Description='Compound' Name='Compound' Date='2020-03-05 18:09:25' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -408,10 +408,10 @@
     <t>kegg.compound::C00022</t>
   </si>
   <si>
-    <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2019-10-10 23:09:02' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables Type='Data' Id='Model' Description='Model' Name='Model' Date='2020-03-05 18:09:25' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables Type='Data' Id='Reaction' Description='Reaction' Name='Reaction' Date='2020-03-05 18:09:25' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>
@@ -1190,7 +1190,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A3:G20"/>
   <hyperlinks>
     <hyperlink ref="A3" location="'!!Compound'!A1" tooltip="Click to view compound" display="'!!Compound'!A1"/>
@@ -1328,15 +1328,15 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A2:E7"/>
   <dataValidations count="5">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!Model:1&quot; or blank." sqref="A3:A7">
-      <formula1>'!Model'!$B$1:$XFD$1</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!!Model:2&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!!Model:2&quot; or blank." sqref="A3:A7">
+      <formula1>'!!Model'!$B$2:$XFD$2</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B3:B7">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." sqref="B3:B7">
       <formula1>1</formula1>
-      <formula2>63</formula2>
+      <formula2>90</formula2>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="C3:C7">
       <formula1>255</formula1>
@@ -1391,11 +1391,11 @@
       <c r="B3" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <dataValidations count="2">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." sqref="B2">
       <formula1>1</formula1>
-      <formula2>63</formula2>
+      <formula2>90</formula2>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3">
       <formula1>255</formula1>
@@ -1498,15 +1498,15 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A2:G4"/>
   <dataValidations count="7">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!Model:1&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!Model:1&quot; or blank." sqref="A3:A4">
-      <formula1>'!Model'!$B$1:$XFD$1</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!!Model:2&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!!Model:2&quot; or blank." sqref="A3:A4">
+      <formula1>'!!Model'!$B$2:$XFD$2</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B3:B4">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Identifier&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Identifier&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 90 characters.&#10;&#10;Value must be unique." sqref="B3:B4">
       <formula1>1</formula1>
-      <formula2>63</formula2>
+      <formula2>90</formula2>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="C3:C4">
       <formula1>255</formula1>

</xml_diff>

<commit_message>
adding table format (row/column) to Workbook output
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data_copy.xlsx
+++ b/examples/biochemical_models/data_copy.xlsx
@@ -264,10 +264,10 @@
     <t>'!!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-09 12:59:52'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Schema' description='Table/model and column/attribute definitions' date='2020-03-09 12:59:52' objTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-09 15:30:10'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-09 15:30:10' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -351,7 +351,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' id='Compound' description='Compound' name='Compound' date='2020-03-09 12:59:52' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' id='Compound' description='Compound' name='Compound' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='row'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -408,10 +408,10 @@
     <t>kegg.compound::C00022</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' id='Model' description='Model' name='Model' date='2020-03-09 12:59:52' objTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' id='Reaction' description='Reaction' name='Reaction' date='2020-03-09 12:59:52' objTablesVersion='0.0.8'</t>
+    <t>!!ObjTables type='Data' id='Model' description='Model' name='Model' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='column'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' id='Reaction' description='Reaction' name='Reaction' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='row'</t>
   </si>
   <si>
     <t>!Equation</t>

</xml_diff>

<commit_message>
adding schema to document, table metdata
</commit_message>
<xml_diff>
--- a/examples/biochemical_models/data_copy.xlsx
+++ b/examples/biochemical_models/data_copy.xlsx
@@ -264,10 +264,10 @@
     <t>'!!Reaction'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-09 15:30:10'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-09 15:30:10' objTablesVersion='0.0.8'</t>
+    <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-09 23:57:34'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-03-09 23:57:34' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -351,7 +351,7 @@
     <t>is_reversible</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' id='Compound' description='Compound' name='Compound' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='row'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Compound' name='Compound' description='Compound' date='2020-03-09 23:57:34' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -408,10 +408,10 @@
     <t>kegg.compound::C00022</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' id='Model' description='Model' name='Model' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='column'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' id='Reaction' description='Reaction' name='Reaction' date='2020-03-09 15:30:10' objTablesVersion='0.0.8' tableFormat='row'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-09 23:57:34' objTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' id='Reaction' name='Reaction' description='Reaction' date='2020-03-09 23:57:34' objTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Equation</t>

</xml_diff>